<commit_message>
Added argparsing so that users can change duration and location in the terminal
</commit_message>
<xml_diff>
--- a/system_output.xlsx
+++ b/system_output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,10 +448,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>13.3</v>
+        <v>15.6</v>
       </c>
       <c r="C2" t="n">
-        <v>78.59999999999999</v>
+        <v>83.3</v>
       </c>
       <c r="D2" t="n">
         <v>26.3</v>
@@ -462,12 +462,40 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>15.7</v>
+        <v>15.8</v>
       </c>
       <c r="C3" t="n">
-        <v>79.59999999999999</v>
+        <v>83.2</v>
       </c>
       <c r="D3" t="n">
+        <v>26.3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B4" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>83.2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>26.3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>83.59999999999999</v>
+      </c>
+      <c r="D5" t="n">
         <v>26.3</v>
       </c>
     </row>

</xml_diff>